<commit_message>
updated admin areas and CSV files
</commit_message>
<xml_diff>
--- a/arc_fima/forms/arc_fima/arc_fima.xlsx
+++ b/arc_fima/forms/arc_fima/arc_fima.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app-designer\app\config\tables\arc_fima\forms\arc_fima\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sunny\Desktop\app-designer\app\config\tables\arc_fima\forms\arc_fima\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="survey" sheetId="2" r:id="rId3"/>
     <sheet name="queries" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="165">
   <si>
     <t>setting_name</t>
   </si>
@@ -359,48 +359,21 @@
     <t>select_one_dropdown</t>
   </si>
   <si>
-    <t>regions_csv</t>
-  </si>
-  <si>
     <t>countries_csv</t>
   </si>
   <si>
     <t>country</t>
   </si>
   <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>province</t>
-  </si>
-  <si>
     <t>Select Country</t>
   </si>
   <si>
-    <t>Select Region/State</t>
-  </si>
-  <si>
-    <t>barangay_village</t>
-  </si>
-  <si>
-    <t>municipality_district</t>
-  </si>
-  <si>
-    <t>Enter Muncipality/District</t>
-  </si>
-  <si>
-    <t>Enter Barangay/Village</t>
-  </si>
-  <si>
     <t>choice_filter</t>
   </si>
   <si>
     <t>choice_item.country === data('country')</t>
   </si>
   <si>
-    <t>Enter province</t>
-  </si>
-  <si>
     <t>query_name</t>
   </si>
   <si>
@@ -417,9 +390,6 @@
   </si>
   <si>
     <t>"countries.csv"</t>
-  </si>
-  <si>
-    <t>"regions.csv"</t>
   </si>
   <si>
     <t>_.chain(context).pluck('country').uniq().map(function(country){
@@ -427,69 +397,141 @@
 }).value()</t>
   </si>
   <si>
+    <t>key_commodity</t>
+  </si>
+  <si>
+    <t>linked_form_id</t>
+  </si>
+  <si>
+    <t>linked_table_id</t>
+  </si>
+  <si>
+    <t>selection</t>
+  </si>
+  <si>
+    <t>selectionArgs</t>
+  </si>
+  <si>
+    <t>newRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t>openRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t>arc_fima_commodity</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Commodity Section:</t>
+  </si>
+  <si>
+    <t>This section is used to gather informatin about key commodities.</t>
+  </si>
+  <si>
+    <t>Make a list of all commodities</t>
+  </si>
+  <si>
+    <t>Add Key Commodity</t>
+  </si>
+  <si>
+    <t>Location_Name=?</t>
+  </si>
+  <si>
+    <t>[data('Location_Name')]</t>
+  </si>
+  <si>
+    <t>{ Location_Name : data('Location_Name')}</t>
+  </si>
+  <si>
+    <t>display.new_instance_label.text</t>
+  </si>
+  <si>
+    <t>Add Key commodity</t>
+  </si>
+  <si>
+    <t>admin1_csv</t>
+  </si>
+  <si>
+    <t>"admin1.csv"</t>
+  </si>
+  <si>
     <t>_.map(context, function(place){
-return { country: place.country, data_value: place.region, display: {title: {text: place.region} } };
+return { country: place.country, data_value: place.admin1, display: {title: {text: place.admin1} } };
 })</t>
   </si>
   <si>
-    <t>key_commodity</t>
-  </si>
-  <si>
-    <t>linked_form_id</t>
-  </si>
-  <si>
-    <t>linked_table_id</t>
-  </si>
-  <si>
-    <t>selection</t>
-  </si>
-  <si>
-    <t>selectionArgs</t>
-  </si>
-  <si>
-    <t>newRowInitialElementKeyToValueMap</t>
-  </si>
-  <si>
-    <t>openRowInitialElementKeyToValueMap</t>
-  </si>
-  <si>
-    <t>arc_fima_commodity</t>
-  </si>
-  <si>
-    <t>{}</t>
-  </si>
-  <si>
-    <t>instance_name</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>Commodity Section:</t>
-  </si>
-  <si>
-    <t>This section is used to gather informatin about key commodities.</t>
-  </si>
-  <si>
-    <t>Make a list of all commodities</t>
-  </si>
-  <si>
-    <t>Add Key Commodity</t>
-  </si>
-  <si>
-    <t>Location_Name=?</t>
-  </si>
-  <si>
-    <t>[data('Location_Name')]</t>
-  </si>
-  <si>
-    <t>{ Location_Name : data('Location_Name')}</t>
-  </si>
-  <si>
-    <t>display.new_instance_label.text</t>
-  </si>
-  <si>
-    <t>Add Key commodity</t>
+    <t>Select Region/State (Admin 1)</t>
+  </si>
+  <si>
+    <t>admin1</t>
+  </si>
+  <si>
+    <t>admin2</t>
+  </si>
+  <si>
+    <t>Enter Province/City/Town (Admin 2)</t>
+  </si>
+  <si>
+    <t>admin2_csv</t>
+  </si>
+  <si>
+    <t>"admin2.csv"</t>
+  </si>
+  <si>
+    <t>_.map(context, function(place){
+return { admin1: place.admin1, data_value: place.admin2, display: {title: {text: place.admin2} } };
+})</t>
+  </si>
+  <si>
+    <t>admin3_csv</t>
+  </si>
+  <si>
+    <t>"admin3.csv"</t>
+  </si>
+  <si>
+    <t>_.map(context, function(place){
+return { admin2: place.admin2, data_value: place.admin3, display: {title: {text: place.admin3} } };
+})</t>
+  </si>
+  <si>
+    <t>admin4_csv</t>
+  </si>
+  <si>
+    <t>"admin4.csv"</t>
+  </si>
+  <si>
+    <t>_.map(context, function(place){
+return { admin3: place.admin3, data_value: place.admin4, display: {title: {text: place.admin4} } };
+})</t>
+  </si>
+  <si>
+    <t>admin3</t>
+  </si>
+  <si>
+    <t>admin4</t>
+  </si>
+  <si>
+    <t>Enter Muncipality/District/County (Admin 3)</t>
+  </si>
+  <si>
+    <t>Enter Barangay/Village/Street (Admin 4)</t>
+  </si>
+  <si>
+    <t>choice_item.admin1 === data('admin1')</t>
+  </si>
+  <si>
+    <t>choice_item.admin2 === data('admin2')</t>
+  </si>
+  <si>
+    <t>choice_item.admin3 === data('admin3')</t>
   </si>
 </sst>
 </file>
@@ -940,7 +982,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -1227,17 +1269,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="4" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.140625" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="56.42578125" customWidth="1"/>
@@ -1275,10 +1318,10 @@
         <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1298,21 +1341,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>109</v>
       </c>
@@ -1320,282 +1354,318 @@
         <v>110</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>109</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>109</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>119</v>
+        <v>148</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>59</v>
+        <v>109</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>160</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>22</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G13" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G17" s="3" t="s">
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G19" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G20" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G28" s="4" t="s">
+    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I30" s="4" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G31" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="4" t="s">
+    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>143</v>
-      </c>
-      <c r="D36" t="s">
-        <v>144</v>
-      </c>
-      <c r="I36" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" t="s">
+        <v>133</v>
+      </c>
+      <c r="I37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>108</v>
       </c>
-      <c r="B37" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" t="s">
-        <v>146</v>
-      </c>
-      <c r="I37" t="s">
-        <v>147</v>
-      </c>
-      <c r="K37" t="s">
-        <v>152</v>
+      <c r="B38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" t="s">
+        <v>135</v>
+      </c>
+      <c r="I38" t="s">
+        <v>136</v>
+      </c>
+      <c r="K38" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1605,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,88 +1697,130 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>126</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>127</v>
       </c>
-      <c r="E1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" t="s">
-        <v>138</v>
-      </c>
       <c r="J1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J7" t="s">
         <v>130</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="J4" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>